<commit_message>
Updated several data sources
</commit_message>
<xml_diff>
--- a/data-raw/Census/StateSummaries/ASPP_data_2012plus/aspp_varxwalk.xlsx
+++ b/data-raw/Census/StateSummaries/ASPP_data_2012plus/aspp_varxwalk.xlsx
@@ -1,30 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\RPrograms PC\Packages\Pensions packages\pdata\data-raw\Census\StateSummaries\ASPP_data_2012plus\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBC334E-BC50-4806-93B1-69ADA6CE0C7D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="60">
   <si>
     <t>Total Contributions</t>
   </si>
@@ -201,12 +207,15 @@
   </si>
   <si>
     <t>var_2016</t>
+  </si>
+  <si>
+    <t>var_2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -552,19 +561,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="56.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -583,8 +595,11 @@
       <c r="F1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>0</v>
@@ -601,8 +616,11 @@
       <c r="F2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
@@ -621,8 +639,11 @@
       <c r="F3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -641,8 +662,11 @@
       <c r="F4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -661,8 +685,11 @@
       <c r="F5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
@@ -681,8 +708,11 @@
       <c r="F6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -701,8 +731,11 @@
       <c r="F7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -721,8 +754,11 @@
       <c r="F8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -741,8 +777,11 @@
       <c r="F9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -761,8 +800,11 @@
       <c r="F10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -781,8 +823,11 @@
       <c r="F11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -801,8 +846,11 @@
       <c r="F12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
@@ -821,8 +869,11 @@
       <c r="F13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
@@ -841,8 +892,11 @@
       <c r="F14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -861,8 +915,11 @@
       <c r="F15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
@@ -881,8 +938,11 @@
       <c r="F16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
@@ -901,8 +961,11 @@
       <c r="F17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -921,8 +984,11 @@
       <c r="F18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -941,8 +1007,11 @@
       <c r="F19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
@@ -961,8 +1030,11 @@
       <c r="F20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
@@ -981,8 +1053,11 @@
       <c r="F21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>47</v>
       </c>
@@ -1001,8 +1076,11 @@
       <c r="F22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -1021,8 +1099,11 @@
       <c r="F23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
@@ -1041,8 +1122,11 @@
       <c r="F24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
@@ -1061,8 +1145,11 @@
       <c r="F25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -1081,8 +1168,11 @@
       <c r="F26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -1101,8 +1191,11 @@
       <c r="F27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1121,8 +1214,11 @@
       <c r="F28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>47</v>
       </c>
@@ -1141,8 +1237,11 @@
       <c r="F29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>47</v>
       </c>
@@ -1161,8 +1260,11 @@
       <c r="F30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>47</v>
       </c>
@@ -1181,8 +1283,11 @@
       <c r="F31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>49</v>
       </c>
@@ -1201,8 +1306,11 @@
       <c r="F32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>50</v>
       </c>
@@ -1221,8 +1329,11 @@
       <c r="F33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>51</v>
       </c>
@@ -1241,8 +1352,11 @@
       <c r="F34" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>52</v>
       </c>
@@ -1261,8 +1375,11 @@
       <c r="F35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
@@ -1281,8 +1398,11 @@
       <c r="F36" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
@@ -1302,7 +1422,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>

</xml_diff>